<commit_message>
add filtering by year for study
</commit_message>
<xml_diff>
--- a/vavilov3/tests/data/excels/studies.xlsx
+++ b/vavilov3/tests/data/excels/studies.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -61,10 +61,10 @@
     <t xml:space="preserve">no</t>
   </si>
   <si>
-    <t xml:space="preserve">17/01/17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/12/01</t>
+    <t xml:space="preserve">2017/01/17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017/12/01</t>
   </si>
   <si>
     <t xml:space="preserve">Valencia</t>
@@ -88,10 +88,10 @@
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">19/01/01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19/12/01</t>
+    <t xml:space="preserve">2019/01/01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019/12/01</t>
   </si>
   <si>
     <t xml:space="preserve">study3</t>
@@ -119,6 +119,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -207,22 +208,21 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>